<commit_message>
Zeitblätter auf Stand gebracht
</commit_message>
<xml_diff>
--- a/Zeitblätter/Jim Frey.xlsx
+++ b/Zeitblätter/Jim Frey.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">Besprechung, Protokoll, TI für cc2650 </t>
+  </si>
+  <si>
+    <t>Doku auf Stand gebracht</t>
   </si>
 </sst>
 </file>
@@ -424,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -617,7 +620,7 @@
         <v>42662</v>
       </c>
       <c r="B22" s="6">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
@@ -628,7 +631,12 @@
         <f t="shared" si="0"/>
         <v>42663</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -717,7 +725,7 @@
       </c>
       <c r="B36" s="8">
         <f>SUM(B5:B34)</f>
-        <v>23.2</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Zeitblatt angepasst, TI I2C RTOS versucht zumlaufen zu bekommen, geht aber aktuell noch nicht Transaction schlägt fehl!
</commit_message>
<xml_diff>
--- a/Zeitblätter/Jim Frey.xlsx
+++ b/Zeitblätter/Jim Frey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Documents\Eigene Daten\#Master_3\S1 Kopplung\GitHub AlienHacky\Zeitblätter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Documents\Eigene Daten\#Master_3\S1_Kopplung\GitHub_AlienHacky\Zeitblätter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Doku auf Stand gebracht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC2650 in betrieb genommen, TI RTOS eingelesen, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC2650 I2C Beispiel laufen lassen, nun spinnt der debugger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C Beispiel geschrieben, gibt fehler beim start der Transaction </t>
   </si>
 </sst>
 </file>
@@ -428,7 +437,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -643,21 +652,36 @@
         <f t="shared" si="0"/>
         <v>42664</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>42665</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>42666</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -725,7 +749,7 @@
       </c>
       <c r="B36" s="8">
         <f>SUM(B5:B34)</f>
-        <v>24.2</v>
+        <v>30.2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Zeitblatt Aktualiesiert Bild für Launchpad CC2650
</commit_message>
<xml_diff>
--- a/Zeitblätter/Jim Frey.xlsx
+++ b/Zeitblätter/Jim Frey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Documents\Eigene Daten\#Master_3\S1 Kopplung\GitHub AlienHacky\Zeitblätter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\GitHub_AlienHacky\Zeitblätter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>Doku auf Stand gebracht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC2650 in betrieb genommen, TI RTOS eingelesen, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C Beispiel geschrieben, gibt fehler beim start der Transaction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC2650 I2C Beispiel laufen lassen, nun spinnt der debugger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O Pins geprüft zwischen CC2650 und Senor Hub, Bild erstellt, wie Pins angepasst werden müssen. Konkret I2C  muss anders liegen, wenn Analog kein interrupt hat muss der Lichtsensor Pin umgelegt werden.  Stecker gesucht und flachbandkabel! </t>
   </si>
 </sst>
 </file>
@@ -427,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -464,7 +476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A4+1</f>
         <v>42645</v>
@@ -558,7 +570,7 @@
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>42656</v>
@@ -643,21 +655,36 @@
         <f t="shared" si="0"/>
         <v>42664</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>42665</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>42666</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -666,12 +693,17 @@
       </c>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>42668</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -725,7 +757,7 @@
       </c>
       <c r="B36" s="8">
         <f>SUM(B5:B34)</f>
-        <v>24.2</v>
+        <v>31.7</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>